<commit_message>
Regretion Run SCD0001, SCD0028, SCD0030, SCD0031, SCD0033
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0033_Validasi Database Table Booster.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0033_Validasi Database Table Booster.xlsx
@@ -5,31 +5,32 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF77FFE-C50C-4F8C-8DD9-F308123D2A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1FB90B-0EE5-420D-9BB5-C1FEC30AC3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0033" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>SIDEBAR_MENU</t>
-  </si>
-  <si>
-    <t>SIDEBAR_SUBMENU</t>
-  </si>
-  <si>
-    <t>SIDEBAR_SUBMENU_SUBMENU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>RUN</t>
   </si>
@@ -69,6 +70,42 @@
   </si>
   <si>
     <t>PASSWORD_DB</t>
+  </si>
+  <si>
+    <t>HOSTNAME</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY1</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY2</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY3</t>
+  </si>
+  <si>
+    <t>QUERY1</t>
+  </si>
+  <si>
+    <t>QUERY2</t>
+  </si>
+  <si>
+    <t>QUERY3</t>
+  </si>
+  <si>
+    <t>DATABASE_1</t>
+  </si>
+  <si>
+    <t>DATABASE_2</t>
+  </si>
+  <si>
+    <t>Digisales_KPI</t>
+  </si>
+  <si>
+    <t>Digisales_SAPM</t>
+  </si>
+  <si>
+    <t>192.168.232.6</t>
   </si>
 </sst>
 </file>
@@ -155,11 +192,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,15 +517,15 @@
     <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.28515625" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1"/>
     <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.7109375" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
@@ -498,65 +535,102 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="G2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="1"/>
+      <c r="H2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="9" t="str">
+        <f>"Menampilkan Semua Data pada dbo.TMP_BOOSTER di Database " &amp; O2</f>
+        <v>Menampilkan Semua Data pada dbo.TMP_BOOSTER di Database Digisales_KPI</v>
+      </c>
+      <c r="J2" s="9" t="str">
+        <f>"Menampilkan Semua Data pada dbo.TMP_BOOSTER di Database " &amp; P2</f>
+        <v>Menampilkan Semua Data pada dbo.TMP_BOOSTER di Database Digisales_SAPM</v>
+      </c>
+      <c r="K2" s="12"/>
+      <c r="L2" s="13" t="str">
+        <f>"USE " &amp; O2 &amp; "; Select * From dbo.TMP_BOOSTER"</f>
+        <v>USE Digisales_KPI; Select * From dbo.TMP_BOOSTER</v>
+      </c>
+      <c r="M2" s="13" t="str">
+        <f>"USE " &amp; P2 &amp; "; Select * From dbo.TMP_BOOSTER"</f>
+        <v>USE Digisales_SAPM; Select * From dbo.TMP_BOOSTER</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>

</xml_diff>